<commit_message>
add List<'Entiti'> findAllById(ArrayList<Long> ids); to repositories, fix delete generic method and add delete functionality to rolFormAction
</commit_message>
<xml_diff>
--- a/spring-social/queries/sentences SQL.xlsx
+++ b/spring-social/queries/sentences SQL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="8">
   <si>
     <t>rol_id</t>
   </si>
@@ -47,7 +47,7 @@
     <t>getDate()</t>
   </si>
   <si>
-    <t>null</t>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -83,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,9 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G42"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -379,1009 +378,1050 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE("(",A2,",",B2,",",C2,",",D2,",",E2,",",F2,"),")</f>
+        <v>(getDate(),NULL,1,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <f>+C2+1</f>
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G42" si="0">CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,"),")</f>
+        <v>(getDate(),NULL,2,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C42" si="1">+C3+1</f>
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>(getDate(),NULL,3,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>(getDate(),NULL,4,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="str">
-        <f>+CONCATENATE("(",A2,",",B2,",",C2,",",D2,",",E2,",",F2,"),")</f>
-        <v>(1,1,0,0,getDate(),null),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G42" si="0">+CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,"),")</f>
-        <v>(1,2,0,0,getDate(),null),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>(1,3,0,0,getDate(),null),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>(1,4,0,0,getDate(),null),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>(1,5,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,5,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>(1,6,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,6,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>(1,7,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,7,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>(1,8,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,8,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>(1,9,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,9,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>(1,10,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,10,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>(1,11,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,11,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>(1,12,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,12,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
         <v>7</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>(1,13,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,13,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
         <v>7</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>(1,14,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,14,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>(1,15,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,15,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
         <v>7</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>(1,16,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,16,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>(1,17,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,17,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>(1,18,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,18,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>(1,19,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,19,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>(1,20,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,20,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
       <c r="D22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>(1,21,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,21,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>(1,22,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,22,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>(1,23,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,23,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>(1,24,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,24,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
         <v>7</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>(1,25,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,25,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
         <v>7</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>(1,26,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,26,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>(1,27,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,27,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29">
+      <c r="A29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>(1,28,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,28,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30">
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F30" t="s">
         <v>7</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>(1,29,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,29,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
         <v>7</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>(1,30,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,30,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32">
+      <c r="A32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>(1,31,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,31,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33">
+      <c r="A33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>(1,32,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,32,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
         <v>7</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>(1,33,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,33,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
         <v>7</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>(1,34,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,34,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
+      <c r="A36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
         <v>7</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>(1,35,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,35,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
         <v>7</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>(1,36,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,36,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38">
+      <c r="A38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>(1,37,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,37,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39">
+      <c r="A39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
         <v>7</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>(1,38,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,38,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40">
+      <c r="A40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>(1,39,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,39,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41">
+      <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>(1,40,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,40,1,NULL,NULL),</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
         <v>7</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>(1,41,0,0,getDate(),null),</v>
+        <v>(getDate(),NULL,41,1,NULL,NULL),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix delete functionality in acciones de roles form
</commit_message>
<xml_diff>
--- a/spring-social/queries/sentences SQL.xlsx
+++ b/spring-social/queries/sentences SQL.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rol_form_action" sheetId="1" r:id="rId1"/>
+    <sheet name="form_action" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="14">
   <si>
     <t>rol_id</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>action_id</t>
+  </si>
+  <si>
+    <t>item_order</t>
+  </si>
+  <si>
+    <t>GETDATE()</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>is_the_rol</t>
   </si>
 </sst>
 </file>
@@ -83,9 +102,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,9 +388,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -395,6 +419,9 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -453,7 +480,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C42" si="1">+C3+1</f>
+        <f t="shared" ref="C4:C50" si="1">+C3+1</f>
         <v>3</v>
       </c>
       <c r="D4">
@@ -1418,10 +1445,1776 @@
       <c r="G42" t="str">
         <f t="shared" si="0"/>
         <v>(getDate(),NULL,41,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" ref="G43:G50" si="2">CONCATENATE("(",A43,",",B43,",",C43,",",D43,",",E43,",",F43,"),")</f>
+        <v>(getDate(),NULL,42,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,43,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,44,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,45,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,46,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,47,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,48,1,NULL,NULL),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="2"/>
+        <v>(getDate(),NULL,49,1,NULL,NULL),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="12.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="49.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <f>+B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE("(",A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,"),")</f>
+        <v>(1,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C50" si="0">+B3</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I50" si="1">CONCATENATE("(",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,"),")</f>
+        <v>(1,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>(1,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>(1,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>(1,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>(1,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>(2,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>(3,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>(4,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>5</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v>(5,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>6</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>6</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>6</v>
+      </c>
+      <c r="B36" s="2">
+        <v>5</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>6</v>
+      </c>
+      <c r="B37" s="2">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>6</v>
+      </c>
+      <c r="B38" s="2">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v>(6,7,7,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2">
+        <v>4</v>
+      </c>
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>7</v>
+      </c>
+      <c r="B43" s="2">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2">
+        <v>6</v>
+      </c>
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v>(7,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>8</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>8</v>
+      </c>
+      <c r="B47" s="2">
+        <v>3</v>
+      </c>
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>8</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4</v>
+      </c>
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>8</v>
+      </c>
+      <c r="B49" s="2">
+        <v>5</v>
+      </c>
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>8</v>
+      </c>
+      <c r="B50" s="2">
+        <v>6</v>
+      </c>
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v>(8,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
split insert first sentences into SQLSERVER and ORACLE files
</commit_message>
<xml_diff>
--- a/spring-social/queries/sentences SQL.xlsx
+++ b/spring-social/queries/sentences SQL.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="rol_form_action" sheetId="1" r:id="rId1"/>
-    <sheet name="form_action" sheetId="2" r:id="rId2"/>
+    <sheet name="rol_form_action SQLSERVER" sheetId="1" r:id="rId1"/>
+    <sheet name="rol_form_action ORACLE" sheetId="4" r:id="rId2"/>
+    <sheet name="form_action SQLSERVER" sheetId="2" r:id="rId3"/>
+    <sheet name="form_action ORACLE" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="16">
   <si>
     <t>rol_id</t>
   </si>
@@ -67,6 +69,12 @@
   </si>
   <si>
     <t>is_the_rol</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss')</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1663,1650 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="str">
+        <f>CONCATENATE("insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (",A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,");")</f>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (1,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,1,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>1+A2</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <f>+D2+1</f>
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H50" si="0">CONCATENATE("insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (",A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,");")</f>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (2,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,2,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A50" si="1">1+A3</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D56" si="2">+D3+1</f>
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (3,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,3,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (4,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,4,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (5,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,5,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (6,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,6,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (7,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,7,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (8,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,8,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (9,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,9,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (10,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,10,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (11,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,11,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (12,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,12,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (13,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,13,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (14,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,14,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (15,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,15,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (16,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,16,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (17,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,17,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (18,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,18,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (19,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,19,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (20,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,20,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (21,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,21,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (22,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,22,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (23,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,23,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (24,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,24,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (25,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,25,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (26,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,26,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (27,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,27,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (28,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,28,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (29,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,29,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (30,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,30,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (31,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,31,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (32,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,32,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (33,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,33,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="s">
+        <v>7</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (34,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,34,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (35,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,35,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (36,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,36,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (37,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,37,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (38,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,38,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (39,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,39,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (40,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,40,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (41,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,41,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (42,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,42,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (43,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,43,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (44,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,44,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (45,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,45,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (46,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,46,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (47,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,47,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (48,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,48,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (49,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,49,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" ref="A51:A56" si="3">1+A50</f>
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" ref="H51:H56" si="4">CONCATENATE("insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (",A51,",",B51,",",C51,",",D51,",",E51,",",F51,",",G51,");")</f>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (50,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,50,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (51,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,51,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (52,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,52,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (53,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,53,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (54,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,54,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (55,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,55,1,NULL,NULL);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,4 +4865,1981 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="12.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="49.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <f>+C2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",A2,",", B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,");")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (1,1,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>+A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D50" si="0">+C3</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J50" si="1">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",A3,",", B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,");")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (2,1,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A56" si="2">+A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (3,1,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (4,1,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (5,1,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (6,1,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (7,2,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (8,2,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (9,2,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (10,2,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (11,2,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (12,2,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (13,3,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (14,3,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (15,3,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (16,3,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (17,3,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (18,3,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (19,4,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (20,4,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (21,4,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (22,4,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (23,4,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (24,4,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (25,5,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (26,5,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (27,5,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (28,5,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (29,5,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>5</v>
+      </c>
+      <c r="C31" s="2">
+        <v>6</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (30,5,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (31,6,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (32,6,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (33,6,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2">
+        <v>4</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (34,6,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (35,6,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (36,6,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2">
+        <v>7</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (37,6,7,7,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>7</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (38,7,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>7</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (39,7,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>7</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (40,7,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>7</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (41,7,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>7</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (42,7,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>7</v>
+      </c>
+      <c r="C44" s="2">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (43,7,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>8</v>
+      </c>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (44,8,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>8</v>
+      </c>
+      <c r="C46" s="2">
+        <v>2</v>
+      </c>
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (45,8,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (46,8,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>8</v>
+      </c>
+      <c r="C48" s="2">
+        <v>4</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (47,8,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>8</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (48,8,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="2">
+        <v>8</v>
+      </c>
+      <c r="C50" s="2">
+        <v>6</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" si="1"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (49,8,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="2">
+        <v>9</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1</v>
+      </c>
+      <c r="D51" s="2">
+        <f t="shared" ref="D51:D56" si="3">+C51</f>
+        <v>1</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" ref="J51:J56" si="4">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",A51,",", B51,",",C51,",",D51,",",E51,",",F51,",",G51,",",H51,",",I51,");")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (50,9,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="2">
+        <v>9</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (51,9,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="2">
+        <v>9</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (52,9,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="2">
+        <v>9</v>
+      </c>
+      <c r="C54" s="2">
+        <v>4</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (53,9,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="2">
+        <v>9</v>
+      </c>
+      <c r="C55" s="2">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (54,9,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="2">
+        <v>9</v>
+      </c>
+      <c r="C56" s="2">
+        <v>6</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" si="4"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,9,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add system to form, formGroup and frontend system
</commit_message>
<xml_diff>
--- a/spring-social/queries/sentences SQL.xlsx
+++ b/spring-social/queries/sentences SQL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7935" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20700" windowHeight="7935" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rol_form_action SQLSERVER" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="16">
   <si>
     <t>rol_id</t>
   </si>
@@ -1663,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H80" sqref="H2:H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1770,7 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D56" si="2">+D3+1</f>
+        <f t="shared" ref="D4:D67" si="2">+D3+1</f>
         <v>3</v>
       </c>
       <c r="E4">
@@ -3123,7 +3123,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" ref="A51:A56" si="3">1+A50</f>
+        <f t="shared" ref="A51:A84" si="3">1+A50</f>
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -3294,6 +3294,714 @@
         <f t="shared" si="4"/>
         <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (55,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,55,1,NULL,NULL);</v>
       </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" ref="H57:H84" si="5">CONCATENATE("insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (",A57,",",B57,",",C57,",",D57,",",E57,",",F57,",",G57,");")</f>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (56,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,56,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (57,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,57,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>7</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (58,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,58,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (59,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,59,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (60,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,60,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (61,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,61,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (62,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,62,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (63,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,63,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" t="s">
+        <v>7</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (64,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,64,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" t="s">
+        <v>7</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (65,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,65,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (66,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,66,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D84" si="6">+D67+1</f>
+        <v>67</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (67,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,67,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" t="s">
+        <v>7</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (68,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,68,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="6"/>
+        <v>69</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (69,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,69,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" t="s">
+        <v>7</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (70,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,70,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="6"/>
+        <v>71</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (71,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,71,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="6"/>
+        <v>72</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" t="s">
+        <v>7</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (72,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,72,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="6"/>
+        <v>73</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" t="s">
+        <v>7</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (73,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,73,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="6"/>
+        <v>74</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (74,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,74,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" t="s">
+        <v>7</v>
+      </c>
+      <c r="H76" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (75,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,75,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" t="s">
+        <v>7</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (76,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,76,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="6"/>
+        <v>77</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (77,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,77,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="3"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (78,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,78,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="6"/>
+        <v>79</v>
+      </c>
+      <c r="E80">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" t="s">
+        <v>7</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" si="5"/>
+        <v>insert into rol_form_action (id,created_at,created_by,form_action_id,rol_id,updated_at,updated_by) values  (79,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,79,1,NULL,NULL);</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3303,10 +4011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4862,6 +5570,197 @@
         <v>(8,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
       </c>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>9</v>
+      </c>
+      <c r="B51" s="2">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2">
+        <f t="shared" ref="C51:C56" si="2">+B51</f>
+        <v>1</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" ref="I51:I56" si="3">CONCATENATE("(",A51,",",B51,",",C51,",",D51,",",E51,",",F51,",",G51,",",H51,"),")</f>
+        <v>(9,1,1,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>9</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="3"/>
+        <v>(9,2,2,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>9</v>
+      </c>
+      <c r="B53" s="2">
+        <v>3</v>
+      </c>
+      <c r="C53" s="2">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="3"/>
+        <v>(9,3,3,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>9</v>
+      </c>
+      <c r="B54" s="2">
+        <v>4</v>
+      </c>
+      <c r="C54" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="3"/>
+        <v>(9,4,4,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>9</v>
+      </c>
+      <c r="B55" s="2">
+        <v>5</v>
+      </c>
+      <c r="C55" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="3"/>
+        <v>(9,5,5,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2">
+        <v>6</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="3"/>
+        <v>(9,6,6,NULL,NULL,GETDATE(),NULL,0),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4869,10 +5768,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4986,7 +5885,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A56" si="2">+A3+1</f>
+        <f t="shared" ref="A4:A67" si="2">+A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
@@ -6836,6 +7735,846 @@
       <c r="J56" t="str">
         <f t="shared" si="4"/>
         <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (55,9,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="2">
+        <v>10</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" ref="D57:D74" si="5">+C57</f>
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" ref="J57:J74" si="6">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",A57,",", B57,",",C57,",",D57,",",E57,",",F57,",",G57,",",H57,",",I57,");")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (56,10,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="2">
+        <v>10</v>
+      </c>
+      <c r="C58" s="2">
+        <v>2</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (57,10,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <v>10</v>
+      </c>
+      <c r="C59" s="2">
+        <v>3</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (58,10,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="2">
+        <v>10</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (59,10,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="2">
+        <v>10</v>
+      </c>
+      <c r="C61" s="2">
+        <v>5</v>
+      </c>
+      <c r="D61" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (60,10,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="2">
+        <v>10</v>
+      </c>
+      <c r="C62" s="2">
+        <v>6</v>
+      </c>
+      <c r="D62" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (61,10,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <v>11</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1</v>
+      </c>
+      <c r="D63" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (62,11,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="2">
+        <v>11</v>
+      </c>
+      <c r="C64" s="2">
+        <v>2</v>
+      </c>
+      <c r="D64" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (63,11,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="2">
+        <v>11</v>
+      </c>
+      <c r="C65" s="2">
+        <v>3</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (64,11,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="2">
+        <v>11</v>
+      </c>
+      <c r="C66" s="2">
+        <v>4</v>
+      </c>
+      <c r="D66" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I66" s="2">
+        <v>0</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (65,11,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="2">
+        <v>11</v>
+      </c>
+      <c r="C67" s="2">
+        <v>5</v>
+      </c>
+      <c r="D67" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (66,11,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" ref="A68:A84" si="7">+A67+1</f>
+        <v>67</v>
+      </c>
+      <c r="B68" s="2">
+        <v>11</v>
+      </c>
+      <c r="C68" s="2">
+        <v>6</v>
+      </c>
+      <c r="D68" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I68" s="2">
+        <v>0</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (67,11,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <v>12</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1</v>
+      </c>
+      <c r="D69" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I69" s="2">
+        <v>0</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (68,12,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="2">
+        <v>12</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2</v>
+      </c>
+      <c r="D70" s="2">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (69,12,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="2">
+        <v>12</v>
+      </c>
+      <c r="C71" s="2">
+        <v>3</v>
+      </c>
+      <c r="D71" s="2">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (70,12,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="2">
+        <v>12</v>
+      </c>
+      <c r="C72" s="2">
+        <v>4</v>
+      </c>
+      <c r="D72" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="2">
+        <v>0</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (71,12,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="2">
+        <v>12</v>
+      </c>
+      <c r="C73" s="2">
+        <v>5</v>
+      </c>
+      <c r="D73" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I73" s="2">
+        <v>0</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (72,12,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="2">
+        <v>12</v>
+      </c>
+      <c r="C74" s="2">
+        <v>6</v>
+      </c>
+      <c r="D74" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I74" s="2">
+        <v>0</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" si="6"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (73,12,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
+        <v>13</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1</v>
+      </c>
+      <c r="D75" s="2">
+        <f t="shared" ref="D75:D80" si="8">+C75</f>
+        <v>1</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" ref="J75:J80" si="9">CONCATENATE("insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (",A75,",", B75,",",C75,",",D75,",",E75,",",F75,",",G75,",",H75,",",I75,");")</f>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (74,13,1,1,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="2">
+        <v>13</v>
+      </c>
+      <c r="C76" s="2">
+        <v>2</v>
+      </c>
+      <c r="D76" s="2">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" s="2">
+        <v>0</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (75,13,2,2,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="2">
+        <v>13</v>
+      </c>
+      <c r="C77" s="2">
+        <v>3</v>
+      </c>
+      <c r="D77" s="2">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="2">
+        <v>0</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (76,13,3,3,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="2">
+        <v>13</v>
+      </c>
+      <c r="C78" s="2">
+        <v>4</v>
+      </c>
+      <c r="D78" s="2">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="2">
+        <v>0</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (77,13,4,4,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="2">
+        <v>13</v>
+      </c>
+      <c r="C79" s="2">
+        <v>5</v>
+      </c>
+      <c r="D79" s="2">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="2">
+        <v>0</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (78,13,5,5,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="2">
+        <v>13</v>
+      </c>
+      <c r="C80" s="2">
+        <v>6</v>
+      </c>
+      <c r="D80" s="2">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I80" s="2">
+        <v>0</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" si="9"/>
+        <v>insert into form_action (id,form_id,action_id,item_order,created_by,updated_by, created_at, updated_at, is_the_rol) values (79,13,6,6,NULL,NULL,TO_CHAR(SYSDATE,'DD/MM/YYYY hh:mm:ss'),NULL,0);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>